<commit_message>
Update Emisiones por Gas 1990-2016 Chile.xlsx
</commit_message>
<xml_diff>
--- a/CHILE/Todos los gases/Emisiones por Gas 1990-2016 Chile.xlsx
+++ b/CHILE/Todos los gases/Emisiones por Gas 1990-2016 Chile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gustavo Arancibia\Dropbox\Diseño DATA's (1)\DATA-ICC\CHILE\Todos los gases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF158149-6B3E-413B-9E16-DE8CF2735E36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0741839-BCDC-40FB-AE1A-96A1B90289AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>CO2</t>
   </si>
@@ -29,12 +29,6 @@
   </si>
   <si>
     <t>N2O</t>
-  </si>
-  <si>
-    <t>HFC</t>
-  </si>
-  <si>
-    <t>SF6</t>
   </si>
   <si>
     <t>CO2eq</t>
@@ -50,12 +44,6 @@
   </si>
   <si>
     <t>Variación N2O</t>
-  </si>
-  <si>
-    <t>Variación HFC</t>
-  </si>
-  <si>
-    <t>Variación SF6</t>
   </si>
   <si>
     <t>Variación CO2eq</t>
@@ -688,7 +676,7 @@
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="32">
+  <dxfs count="28">
     <dxf>
       <font>
         <b val="0"/>
@@ -706,7 +694,27 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0000000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -766,6 +774,26 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="0.0000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -806,7 +834,67 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="164" formatCode="0.0000000"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0000000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -926,126 +1014,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="164" formatCode="0.0000000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0000000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0000000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0000000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0000000"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <numFmt numFmtId="2" formatCode="0.00"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1126,67 +1094,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="164" formatCode="0.0000000"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1343,81 +1251,69 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A62E7D1-6E1A-4CB3-AE37-B2B441D5A2C8}" name="Todo_Gases_Chile" displayName="Todo_Gases_Chile" ref="A2:AD29" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
-  <autoFilter ref="A2:AD29" xr:uid="{B70683CC-222B-4197-BEBB-B08A8E7898CC}"/>
-  <tableColumns count="30">
-    <tableColumn id="1" xr3:uid="{7158FBDF-FEA3-471B-A42C-92B89F393C25}" name="Año" dataDxfId="29"/>
-    <tableColumn id="2" xr3:uid="{F7BF00BC-E481-4FB7-974C-A25EBC237A54}" name="CO2" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{ED3D2D64-98C8-4B1C-AED5-77E1D346BAEE}" name="CO2 (CO2eq)" dataDxfId="9"/>
-    <tableColumn id="9" xr3:uid="{72AD2C7F-8A4D-4C89-9D9E-03AFD0C5A6EE}" name="Variación Anual CO2" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A62E7D1-6E1A-4CB3-AE37-B2B441D5A2C8}" name="Todo_Gases_Chile" displayName="Todo_Gases_Chile" ref="A2:Z29" totalsRowShown="0" headerRowDxfId="27" dataDxfId="26">
+  <autoFilter ref="A2:Z29" xr:uid="{B70683CC-222B-4197-BEBB-B08A8E7898CC}"/>
+  <tableColumns count="26">
+    <tableColumn id="1" xr3:uid="{7158FBDF-FEA3-471B-A42C-92B89F393C25}" name="Año" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{F7BF00BC-E481-4FB7-974C-A25EBC237A54}" name="CO2" dataDxfId="24"/>
+    <tableColumn id="8" xr3:uid="{ED3D2D64-98C8-4B1C-AED5-77E1D346BAEE}" name="CO2 (CO2eq)" dataDxfId="23"/>
+    <tableColumn id="9" xr3:uid="{72AD2C7F-8A4D-4C89-9D9E-03AFD0C5A6EE}" name="Variación Anual CO2" dataDxfId="22">
       <calculatedColumnFormula>IFERROR(Todo_Gases_Chile[[#This Row],[CO2]]-B2,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{50C21A66-C62B-4967-829F-20ABB479E2B1}" name="Variación Anual CO2 (CO2eq)" dataDxfId="8">
+    <tableColumn id="22" xr3:uid="{50C21A66-C62B-4967-829F-20ABB479E2B1}" name="Variación Anual CO2 (CO2eq)" dataDxfId="21">
       <calculatedColumnFormula>IFERROR(Todo_Gases_Chile[[#This Row],[CO2 (CO2eq)]]-C2,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{65CC7CEF-FE7C-462E-8843-95FEB3701EFA}" name="CO2 per cápita" dataDxfId="14">
+    <tableColumn id="16" xr3:uid="{65CC7CEF-FE7C-462E-8843-95FEB3701EFA}" name="CO2 per cápita" dataDxfId="20">
       <calculatedColumnFormula>(Todo_Gases_Chile[[#This Row],[CO2]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B1469A0C-13B9-4DC0-9AE8-84E502D39DF6}" name="CH4" dataDxfId="26"/>
-    <tableColumn id="23" xr3:uid="{68578F54-3D77-421C-BD09-AE7CBA0B2721}" name="CH4 (CO2eq)" dataDxfId="7">
+    <tableColumn id="3" xr3:uid="{B1469A0C-13B9-4DC0-9AE8-84E502D39DF6}" name="CH4" dataDxfId="19"/>
+    <tableColumn id="23" xr3:uid="{68578F54-3D77-421C-BD09-AE7CBA0B2721}" name="CH4 (CO2eq)" dataDxfId="18">
       <calculatedColumnFormula>Todo_Gases_Chile[[#This Row],[CH4]]*25</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{76A3A978-B1CB-4056-9C55-50B202E177CA}" name="Variación CH4" dataDxfId="25">
+    <tableColumn id="10" xr3:uid="{76A3A978-B1CB-4056-9C55-50B202E177CA}" name="Variación CH4" dataDxfId="17">
       <calculatedColumnFormula>IFERROR(Todo_Gases_Chile[[#This Row],[CH4]]-G2,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{7572F078-815B-4860-9ADB-7779642E320B}" name="Variación CH4 (CO2eq)" dataDxfId="6">
+    <tableColumn id="24" xr3:uid="{7572F078-815B-4860-9ADB-7779642E320B}" name="Variación CH4 (CO2eq)" dataDxfId="16">
       <calculatedColumnFormula>Todo_Gases_Chile[[#This Row],[Variación CH4]]*25</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="17" xr3:uid="{6066960E-1D3E-4D08-A15D-8F20C2F1C37B}" name="CH4 per cápita" dataDxfId="15">
       <calculatedColumnFormula>(Todo_Gases_Chile[[#This Row],[CH4]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AA1635BE-D69C-4432-920F-F6374432728C}" name="N2O" dataDxfId="24"/>
-    <tableColumn id="25" xr3:uid="{A454B457-35E4-4DA8-A3CC-54BA3D41F6A7}" name="N2O (CO2eq)" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{AA1635BE-D69C-4432-920F-F6374432728C}" name="N2O" dataDxfId="14"/>
+    <tableColumn id="25" xr3:uid="{A454B457-35E4-4DA8-A3CC-54BA3D41F6A7}" name="N2O (CO2eq)" dataDxfId="13">
       <calculatedColumnFormula>Todo_Gases_Chile[[#This Row],[N2O]]*298</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{9505DA53-C20A-4828-AC82-DC4957809C0F}" name="Variación N2O" dataDxfId="23">
+    <tableColumn id="11" xr3:uid="{9505DA53-C20A-4828-AC82-DC4957809C0F}" name="Variación N2O" dataDxfId="12">
       <calculatedColumnFormula>IFERROR(Todo_Gases_Chile[[#This Row],[N2O]]-L2,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{546C1A59-CC95-4396-8E6B-B1C898BF8C05}" name="Variación N2O (CO2eq)" dataDxfId="4">
+    <tableColumn id="26" xr3:uid="{546C1A59-CC95-4396-8E6B-B1C898BF8C05}" name="Variación N2O (CO2eq)" dataDxfId="11">
       <calculatedColumnFormula>Todo_Gases_Chile[[#This Row],[Variación N2O]]*298</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{86CD1BA9-884B-46AA-A2F4-344BC73776CD}" name="N2O per cápita" dataDxfId="13">
+    <tableColumn id="18" xr3:uid="{86CD1BA9-884B-46AA-A2F4-344BC73776CD}" name="N2O per cápita" dataDxfId="10">
       <calculatedColumnFormula>(Todo_Gases_Chile[[#This Row],[N2O]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" xr3:uid="{5D683973-1FDA-4FAB-BA15-842122FFB471}" name="HFC" dataDxfId="22"/>
-    <tableColumn id="27" xr3:uid="{D057883A-1329-41C6-B5C6-A8F9AA81E082}" name="HFC (CO2eq)" dataDxfId="3">
-      <calculatedColumnFormula>Todo_Gases_Chile[[#This Row],[HFC]]*7400</calculatedColumnFormula>
+    <tableColumn id="5" xr3:uid="{5D683973-1FDA-4FAB-BA15-842122FFB471}" name="HFC (CO2eq)" dataDxfId="9"/>
+    <tableColumn id="12" xr3:uid="{C48DE327-A905-49E6-947F-04DB1AAD67DA}" name="Variación HFC (CO2eq)" dataDxfId="8">
+      <calculatedColumnFormula>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q2,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{C48DE327-A905-49E6-947F-04DB1AAD67DA}" name="Variación HFC" dataDxfId="21">
-      <calculatedColumnFormula>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q2,"")</calculatedColumnFormula>
+    <tableColumn id="19" xr3:uid="{80E34099-D465-4BDA-A5F0-489FDE91E75C}" name="HFC per cápita" dataDxfId="7">
+      <calculatedColumnFormula>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{F9027973-7EC3-4A48-ADBC-75B0EEB1D87C}" name="Variación HFC (CO2eq)" dataDxfId="2">
-      <calculatedColumnFormula>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</calculatedColumnFormula>
+    <tableColumn id="6" xr3:uid="{52A66CD1-361C-4E7F-98B3-EFF35B84353E}" name="SF6 (CO2eq)" dataDxfId="6"/>
+    <tableColumn id="13" xr3:uid="{0CE9F65F-5906-41AE-88CD-AE9BCF01BA01}" name="Variación SF6 (CO2eq)" dataDxfId="5">
+      <calculatedColumnFormula>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T2,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{80E34099-D465-4BDA-A5F0-489FDE91E75C}" name="HFC per cápita" dataDxfId="12">
-      <calculatedColumnFormula>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</calculatedColumnFormula>
+    <tableColumn id="20" xr3:uid="{3ED8E3C7-5611-421C-ACA5-C1D3E5798319}" name="SF6 per cápita" dataDxfId="4">
+      <calculatedColumnFormula>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{52A66CD1-361C-4E7F-98B3-EFF35B84353E}" name="SF6" dataDxfId="20"/>
-    <tableColumn id="29" xr3:uid="{0EC42475-020B-41C4-9C10-52EAA68126BD}" name="SF6 (CO2eq)" dataDxfId="1">
-      <calculatedColumnFormula>Todo_Gases_Chile[[#This Row],[SF6]]*22800</calculatedColumnFormula>
+    <tableColumn id="7" xr3:uid="{1B015680-EBF5-4DEF-8D0E-8AC8104F202C}" name="CO2eq" dataDxfId="3"/>
+    <tableColumn id="14" xr3:uid="{71C247BD-4FE6-493B-9C57-DCCBD431BB2B}" name="Variación CO2eq" dataDxfId="2">
+      <calculatedColumnFormula>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W2,"")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{0CE9F65F-5906-41AE-88CD-AE9BCF01BA01}" name="Variación SF6" dataDxfId="19">
-      <calculatedColumnFormula>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V2,"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="30" xr3:uid="{9D8D21E5-EE8A-4197-980A-5908904E580E}" name="Variación SF6 (CO2eq)" dataDxfId="0">
-      <calculatedColumnFormula>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="20" xr3:uid="{3ED8E3C7-5611-421C-ACA5-C1D3E5798319}" name="SF6 per cápita" dataDxfId="11">
-      <calculatedColumnFormula>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="7" xr3:uid="{1B015680-EBF5-4DEF-8D0E-8AC8104F202C}" name="CO2eq" dataDxfId="18"/>
-    <tableColumn id="14" xr3:uid="{71C247BD-4FE6-493B-9C57-DCCBD431BB2B}" name="Variación CO2eq" dataDxfId="17">
-      <calculatedColumnFormula>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA2,"")</calculatedColumnFormula>
-    </tableColumn>
-    <tableColumn id="21" xr3:uid="{923547CB-9689-4417-AC25-B9D303EBFE93}" name="CO2eq per cápita" dataDxfId="10">
+    <tableColumn id="21" xr3:uid="{923547CB-9689-4417-AC25-B9D303EBFE93}" name="CO2eq per cápita" dataDxfId="1">
       <calculatedColumnFormula>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{07ACE464-88E8-4806-8DCD-D8EAF152256A}" name="Población" dataDxfId="16"/>
+    <tableColumn id="15" xr3:uid="{07ACE464-88E8-4806-8DCD-D8EAF152256A}" name="Población" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1720,10 +1616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BH49"/>
+  <dimension ref="A1:BD49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1745,23 +1641,19 @@
     <col min="15" max="15" width="12.7109375" style="4" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="10.7109375" style="3" customWidth="1"/>
     <col min="17" max="17" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.7109375" style="3" customWidth="1"/>
-    <col min="22" max="22" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="10.7109375" style="3" customWidth="1"/>
-    <col min="27" max="27" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="12.7109375" style="3" customWidth="1"/>
+    <col min="18" max="18" width="12.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.7109375" style="3" customWidth="1"/>
+    <col min="20" max="20" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" style="3" customWidth="1"/>
+    <col min="23" max="23" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -1785,102 +1677,90 @@
       <c r="U1" s="9"/>
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
     </row>
-    <row r="2" spans="1:60" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:56" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="U2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="X2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Y2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AB2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AC2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AD2" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="AC2" s="3"/>
+      <c r="AD2" s="3"/>
+      <c r="AE2" s="3"/>
+      <c r="AF2" s="3"/>
       <c r="AG2" s="3"/>
       <c r="AH2" s="3"/>
       <c r="AI2" s="3"/>
@@ -1905,12 +1785,8 @@
       <c r="BB2" s="3"/>
       <c r="BC2" s="3"/>
       <c r="BD2" s="3"/>
-      <c r="BE2" s="3"/>
-      <c r="BF2" s="3"/>
-      <c r="BG2" s="3"/>
-      <c r="BH2" s="3"/>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1990</v>
       </c>
@@ -1973,55 +1849,43 @@
       <c r="Q3" s="5">
         <v>0</v>
       </c>
-      <c r="R3" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
+      <c r="R3" s="5" t="str">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q2,"")</f>
+        <v/>
+      </c>
+      <c r="S3" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>0</v>
       </c>
-      <c r="S3" s="5" t="str">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q2,"")</f>
+      <c r="T3" s="5">
+        <v>61.328415900000003</v>
+      </c>
+      <c r="U3" s="5" t="str">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T2,"")</f>
         <v/>
       </c>
-      <c r="T3" s="5" t="e">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="U3" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="V3" s="5">
-        <v>61.328415900000003</v>
+      <c r="V3" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>4.6534954017755519</v>
       </c>
       <c r="W3" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>1398287.88252</v>
+        <v>1954.9669484999999</v>
       </c>
       <c r="X3" s="5" t="str">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V2,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W2,"")</f>
         <v/>
       </c>
-      <c r="Y3" s="5" t="e">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Z3" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>4.6534954017755519</v>
-      </c>
-      <c r="AA3" s="5">
-        <v>1954.9669484999999</v>
-      </c>
-      <c r="AB3" s="5" t="str">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA2,"")</f>
-        <v/>
-      </c>
-      <c r="AC3" s="7">
+      <c r="Y3" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>148.33955144548145</v>
       </c>
-      <c r="AD3" s="6">
+      <c r="Z3" s="6">
         <v>13179000</v>
       </c>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
       <c r="AG3" s="3"/>
       <c r="AH3" s="3"/>
       <c r="AI3" s="3"/>
@@ -2040,12 +1904,8 @@
       <c r="AV3" s="3"/>
       <c r="AW3" s="3"/>
       <c r="AX3" s="3"/>
-      <c r="AY3" s="3"/>
-      <c r="AZ3" s="3"/>
-      <c r="BA3" s="3"/>
-      <c r="BB3" s="3"/>
     </row>
-    <row r="4" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1991</v>
       </c>
@@ -2109,54 +1969,42 @@
         <v>0</v>
       </c>
       <c r="R4" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q3,"")</f>
         <v>0</v>
       </c>
-      <c r="S4" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q3,"")</f>
+      <c r="S4" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>0</v>
       </c>
       <c r="T4" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>0</v>
-      </c>
-      <c r="U4" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="V4" s="5">
         <v>43.749966899999997</v>
       </c>
+      <c r="U4" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T3,"")</f>
+        <v>-17.578449000000006</v>
+      </c>
+      <c r="V4" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>3.2595713679034422</v>
+      </c>
       <c r="W4" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>997499.24531999987</v>
+        <v>4463.4610482999997</v>
       </c>
       <c r="X4" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V3,"")</f>
-        <v>-17.578449000000006</v>
-      </c>
-      <c r="Y4" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>-400788.63720000011</v>
-      </c>
-      <c r="Z4" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>3.2595713679034422</v>
-      </c>
-      <c r="AA4" s="5">
-        <v>4463.4610482999997</v>
-      </c>
-      <c r="AB4" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA3,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W3,"")</f>
         <v>2508.4940997999997</v>
       </c>
-      <c r="AC4" s="7">
+      <c r="Y4" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>332.54813353449561</v>
       </c>
-      <c r="AD4" s="6">
+      <c r="Z4" s="6">
         <v>13422000</v>
       </c>
+      <c r="AC4" s="3"/>
+      <c r="AD4" s="3"/>
+      <c r="AE4" s="3"/>
+      <c r="AF4" s="3"/>
       <c r="AG4" s="3"/>
       <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
@@ -2175,12 +2023,8 @@
       <c r="AV4" s="3"/>
       <c r="AW4" s="3"/>
       <c r="AX4" s="3"/>
-      <c r="AY4" s="3"/>
-      <c r="AZ4" s="3"/>
-      <c r="BA4" s="3"/>
-      <c r="BB4" s="3"/>
     </row>
-    <row r="5" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1992</v>
       </c>
@@ -2244,54 +2088,42 @@
         <v>0</v>
       </c>
       <c r="R5" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q4,"")</f>
         <v>0</v>
       </c>
-      <c r="S5" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q4,"")</f>
+      <c r="S5" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>0</v>
       </c>
       <c r="T5" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>0</v>
-      </c>
-      <c r="U5" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="V5" s="5">
         <v>49.370166900000001</v>
       </c>
+      <c r="U5" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T4,"")</f>
+        <v>5.6202000000000041</v>
+      </c>
+      <c r="V5" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>3.5939392935694694</v>
+      </c>
       <c r="W5" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>1125639.80532</v>
+        <v>3258.0773009</v>
       </c>
       <c r="X5" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V4,"")</f>
-        <v>5.6202000000000041</v>
-      </c>
-      <c r="Y5" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>128140.5600000001</v>
-      </c>
-      <c r="Z5" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>3.5939392935694694</v>
-      </c>
-      <c r="AA5" s="5">
-        <v>3258.0773009</v>
-      </c>
-      <c r="AB5" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA4,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W4,"")</f>
         <v>-1205.3837473999997</v>
       </c>
-      <c r="AC5" s="7">
+      <c r="Y5" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>237.17424445634734</v>
       </c>
-      <c r="AD5" s="6">
+      <c r="Z5" s="6">
         <v>13737062</v>
       </c>
+      <c r="AC5" s="3"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="3"/>
+      <c r="AF5" s="3"/>
       <c r="AG5" s="3"/>
       <c r="AH5" s="3"/>
       <c r="AI5" s="3"/>
@@ -2310,12 +2142,8 @@
       <c r="AV5" s="3"/>
       <c r="AW5" s="3"/>
       <c r="AX5" s="3"/>
-      <c r="AY5" s="3"/>
-      <c r="AZ5" s="3"/>
-      <c r="BA5" s="3"/>
-      <c r="BB5" s="3"/>
     </row>
-    <row r="6" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1993</v>
       </c>
@@ -2379,54 +2207,42 @@
         <v>0</v>
       </c>
       <c r="R6" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q5,"")</f>
         <v>0</v>
       </c>
-      <c r="S6" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q5,"")</f>
+      <c r="S6" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>0</v>
       </c>
       <c r="T6" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>0</v>
-      </c>
-      <c r="U6" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="V6" s="5">
         <v>46.590830599999997</v>
       </c>
+      <c r="U6" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T5,"")</f>
+        <v>-2.7793363000000042</v>
+      </c>
+      <c r="V6" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>3.3382253883170354</v>
+      </c>
       <c r="W6" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>1062270.93768</v>
+        <v>6155.4744505999997</v>
       </c>
       <c r="X6" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V5,"")</f>
-        <v>-2.7793363000000042</v>
-      </c>
-      <c r="Y6" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>-63368.867640000099</v>
-      </c>
-      <c r="Z6" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>3.3382253883170354</v>
-      </c>
-      <c r="AA6" s="5">
-        <v>6155.4744505999997</v>
-      </c>
-      <c r="AB6" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA5,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W5,"")</f>
         <v>2897.3971496999998</v>
       </c>
-      <c r="AC6" s="7">
+      <c r="Y6" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>441.03873709711831</v>
       </c>
-      <c r="AD6" s="6">
+      <c r="Z6" s="6">
         <v>13956766</v>
       </c>
+      <c r="AC6" s="3"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="3"/>
+      <c r="AF6" s="3"/>
       <c r="AG6" s="3"/>
       <c r="AH6" s="3"/>
       <c r="AI6" s="3"/>
@@ -2445,12 +2261,8 @@
       <c r="AV6" s="3"/>
       <c r="AW6" s="3"/>
       <c r="AX6" s="3"/>
-      <c r="AY6" s="3"/>
-      <c r="AZ6" s="3"/>
-      <c r="BA6" s="3"/>
-      <c r="BB6" s="3"/>
     </row>
-    <row r="7" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1994</v>
       </c>
@@ -2514,54 +2326,42 @@
         <v>0</v>
       </c>
       <c r="R7" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q6,"")</f>
         <v>0</v>
       </c>
-      <c r="S7" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q6,"")</f>
+      <c r="S7" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>0</v>
       </c>
       <c r="T7" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>0</v>
-      </c>
-      <c r="U7" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="V7" s="5">
         <v>69.843912200000005</v>
       </c>
+      <c r="U7" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T6,"")</f>
+        <v>23.253081600000009</v>
+      </c>
+      <c r="V7" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>4.9283653949622996</v>
+      </c>
       <c r="W7" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>1592441.1981600001</v>
+        <v>12490.632773200001</v>
       </c>
       <c r="X7" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V6,"")</f>
-        <v>23.253081600000009</v>
-      </c>
-      <c r="Y7" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>530170.26048000017</v>
-      </c>
-      <c r="Z7" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>4.9283653949622996</v>
-      </c>
-      <c r="AA7" s="5">
-        <v>12490.632773200001</v>
-      </c>
-      <c r="AB7" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA6,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W6,"")</f>
         <v>6335.1583226000012</v>
       </c>
-      <c r="AC7" s="7">
+      <c r="Y7" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>881.37105127139273</v>
       </c>
-      <c r="AD7" s="6">
+      <c r="Z7" s="6">
         <v>14171821</v>
       </c>
+      <c r="AC7" s="3"/>
+      <c r="AD7" s="3"/>
+      <c r="AE7" s="3"/>
+      <c r="AF7" s="3"/>
       <c r="AG7" s="3"/>
       <c r="AH7" s="3"/>
       <c r="AI7" s="3"/>
@@ -2580,12 +2380,8 @@
       <c r="AV7" s="3"/>
       <c r="AW7" s="3"/>
       <c r="AX7" s="3"/>
-      <c r="AY7" s="3"/>
-      <c r="AZ7" s="3"/>
-      <c r="BA7" s="3"/>
-      <c r="BB7" s="3"/>
     </row>
-    <row r="8" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1995</v>
       </c>
@@ -2649,54 +2445,42 @@
         <v>0</v>
       </c>
       <c r="R8" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q7,"")</f>
         <v>0</v>
       </c>
-      <c r="S8" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q7,"")</f>
+      <c r="S8" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>0</v>
       </c>
       <c r="T8" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>0</v>
-      </c>
-      <c r="U8" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="V8" s="5">
         <v>76.477482699999996</v>
       </c>
+      <c r="U8" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T7,"")</f>
+        <v>6.6335704999999905</v>
+      </c>
+      <c r="V8" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>5.3178609660398752</v>
+      </c>
       <c r="W8" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>1743686.6055599998</v>
+        <v>9371.3739504999994</v>
       </c>
       <c r="X8" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V7,"")</f>
-        <v>6.6335704999999905</v>
-      </c>
-      <c r="Y8" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>151245.40739999979</v>
-      </c>
-      <c r="Z8" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>5.3178609660398752</v>
-      </c>
-      <c r="AA8" s="5">
-        <v>9371.3739504999994</v>
-      </c>
-      <c r="AB8" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA7,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W7,"")</f>
         <v>-3119.2588227000015</v>
       </c>
-      <c r="AC8" s="7">
+      <c r="Y8" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>651.63839041379504</v>
       </c>
-      <c r="AD8" s="6">
+      <c r="Z8" s="6">
         <v>14381249</v>
       </c>
+      <c r="AC8" s="3"/>
+      <c r="AD8" s="3"/>
+      <c r="AE8" s="3"/>
+      <c r="AF8" s="3"/>
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
       <c r="AI8" s="3"/>
@@ -2715,12 +2499,8 @@
       <c r="AV8" s="3"/>
       <c r="AW8" s="3"/>
       <c r="AX8" s="3"/>
-      <c r="AY8" s="3"/>
-      <c r="AZ8" s="3"/>
-      <c r="BA8" s="3"/>
-      <c r="BB8" s="3"/>
     </row>
-    <row r="9" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1996</v>
       </c>
@@ -2784,54 +2564,42 @@
         <v>0</v>
       </c>
       <c r="R9" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q8,"")</f>
         <v>0</v>
       </c>
-      <c r="S9" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q8,"")</f>
+      <c r="S9" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>0</v>
       </c>
       <c r="T9" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>0</v>
-      </c>
-      <c r="U9" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="V9" s="5">
         <v>74.752479600000001</v>
       </c>
+      <c r="U9" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T8,"")</f>
+        <v>-1.725003099999995</v>
+      </c>
+      <c r="V9" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>5.1253171917594216</v>
+      </c>
       <c r="W9" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>1704356.5348799999</v>
+        <v>16447.604175799999</v>
       </c>
       <c r="X9" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V8,"")</f>
-        <v>-1.725003099999995</v>
-      </c>
-      <c r="Y9" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>-39330.070679999888</v>
-      </c>
-      <c r="Z9" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>5.1253171917594216</v>
-      </c>
-      <c r="AA9" s="5">
-        <v>16447.604175799999</v>
-      </c>
-      <c r="AB9" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA8,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W8,"")</f>
         <v>7076.2302252999998</v>
       </c>
-      <c r="AC9" s="7">
+      <c r="Y9" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>1127.710932086349</v>
       </c>
-      <c r="AD9" s="6">
+      <c r="Z9" s="6">
         <v>14584947</v>
       </c>
+      <c r="AC9" s="3"/>
+      <c r="AD9" s="3"/>
+      <c r="AE9" s="3"/>
+      <c r="AF9" s="3"/>
       <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
       <c r="AI9" s="3"/>
@@ -2850,12 +2618,8 @@
       <c r="AV9" s="3"/>
       <c r="AW9" s="3"/>
       <c r="AX9" s="3"/>
-      <c r="AY9" s="3"/>
-      <c r="AZ9" s="3"/>
-      <c r="BA9" s="3"/>
-      <c r="BB9" s="3"/>
     </row>
-    <row r="10" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1997</v>
       </c>
@@ -2919,54 +2683,42 @@
         <v>0</v>
       </c>
       <c r="R10" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q9,"")</f>
         <v>0</v>
       </c>
-      <c r="S10" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q9,"")</f>
+      <c r="S10" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>0</v>
       </c>
       <c r="T10" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>0</v>
-      </c>
-      <c r="U10" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="V10" s="5">
         <v>99.003165699999997</v>
       </c>
+      <c r="U10" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T9,"")</f>
+        <v>24.250686099999996</v>
+      </c>
+      <c r="V10" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>6.697228890299245</v>
+      </c>
       <c r="W10" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>2257272.17796</v>
+        <v>20846.798524099999</v>
       </c>
       <c r="X10" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V9,"")</f>
-        <v>24.250686099999996</v>
-      </c>
-      <c r="Y10" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>552915.64307999995</v>
-      </c>
-      <c r="Z10" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>6.697228890299245</v>
-      </c>
-      <c r="AA10" s="5">
-        <v>20846.798524099999</v>
-      </c>
-      <c r="AB10" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA9,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W9,"")</f>
         <v>4399.1943482999995</v>
       </c>
-      <c r="AC10" s="7">
+      <c r="Y10" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>1410.2153235070764</v>
       </c>
-      <c r="AD10" s="6">
+      <c r="Z10" s="6">
         <v>14782706</v>
       </c>
+      <c r="AC10" s="3"/>
+      <c r="AD10" s="3"/>
+      <c r="AE10" s="3"/>
+      <c r="AF10" s="3"/>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
@@ -2985,12 +2737,8 @@
       <c r="AV10" s="3"/>
       <c r="AW10" s="3"/>
       <c r="AX10" s="3"/>
-      <c r="AY10" s="3"/>
-      <c r="AZ10" s="3"/>
-      <c r="BA10" s="3"/>
-      <c r="BB10" s="3"/>
     </row>
-    <row r="11" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1998</v>
       </c>
@@ -3054,54 +2802,42 @@
         <v>0</v>
       </c>
       <c r="R11" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q10,"")</f>
         <v>0</v>
       </c>
-      <c r="S11" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q10,"")</f>
+      <c r="S11" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>0</v>
       </c>
       <c r="T11" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>0</v>
-      </c>
-      <c r="U11" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>0</v>
-      </c>
-      <c r="V11" s="5">
         <v>122.3586427</v>
       </c>
+      <c r="U11" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T10,"")</f>
+        <v>23.355477000000008</v>
+      </c>
+      <c r="V11" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>8.1709166032383003</v>
+      </c>
       <c r="W11" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>2789777.0535599999</v>
+        <v>39679.775741799996</v>
       </c>
       <c r="X11" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V10,"")</f>
-        <v>23.355477000000008</v>
-      </c>
-      <c r="Y11" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>532504.87560000014</v>
-      </c>
-      <c r="Z11" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>8.1709166032383003</v>
-      </c>
-      <c r="AA11" s="5">
-        <v>39679.775741799996</v>
-      </c>
-      <c r="AB11" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA10,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W10,"")</f>
         <v>18832.977217699998</v>
       </c>
-      <c r="AC11" s="7">
+      <c r="Y11" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>2649.7526555306085</v>
       </c>
-      <c r="AD11" s="6">
+      <c r="Z11" s="6">
         <v>14974898</v>
       </c>
+      <c r="AC11" s="3"/>
+      <c r="AD11" s="3"/>
+      <c r="AE11" s="3"/>
+      <c r="AF11" s="3"/>
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
       <c r="AI11" s="3"/>
@@ -3120,12 +2856,8 @@
       <c r="AV11" s="3"/>
       <c r="AW11" s="3"/>
       <c r="AX11" s="3"/>
-      <c r="AY11" s="3"/>
-      <c r="AZ11" s="3"/>
-      <c r="BA11" s="3"/>
-      <c r="BB11" s="3"/>
     </row>
-    <row r="12" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>1999</v>
       </c>
@@ -3189,54 +2921,42 @@
         <v>38.329203200000002</v>
       </c>
       <c r="R12" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>283636.10368</v>
-      </c>
-      <c r="S12" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q11,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q11,"")</f>
         <v>38.329203200000002</v>
       </c>
+      <c r="S12" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>2.5279191956551861</v>
+      </c>
       <c r="T12" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>283636.10368</v>
-      </c>
-      <c r="U12" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>2.5279191956551861</v>
-      </c>
-      <c r="V12" s="5">
         <v>103.1320956</v>
       </c>
+      <c r="U12" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T11,"")</f>
+        <v>-19.226547100000005</v>
+      </c>
+      <c r="V12" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>6.8018529577830034</v>
+      </c>
       <c r="W12" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>2351411.7796800002</v>
+        <v>30068.488550099999</v>
       </c>
       <c r="X12" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V11,"")</f>
-        <v>-19.226547100000005</v>
-      </c>
-      <c r="Y12" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>-438365.27388000011</v>
-      </c>
-      <c r="Z12" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>6.8018529577830034</v>
-      </c>
-      <c r="AA12" s="5">
-        <v>30068.488550099999</v>
-      </c>
-      <c r="AB12" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA11,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W11,"")</f>
         <v>-9611.2871916999975</v>
       </c>
-      <c r="AC12" s="7">
+      <c r="Y12" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>1983.1017356013278</v>
       </c>
-      <c r="AD12" s="6">
+      <c r="Z12" s="6">
         <v>15162353</v>
       </c>
+      <c r="AC12" s="3"/>
+      <c r="AD12" s="3"/>
+      <c r="AE12" s="3"/>
+      <c r="AF12" s="3"/>
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
       <c r="AI12" s="3"/>
@@ -3255,12 +2975,8 @@
       <c r="AV12" s="3"/>
       <c r="AW12" s="3"/>
       <c r="AX12" s="3"/>
-      <c r="AY12" s="3"/>
-      <c r="AZ12" s="3"/>
-      <c r="BA12" s="3"/>
-      <c r="BB12" s="3"/>
     </row>
-    <row r="13" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2000</v>
       </c>
@@ -3324,54 +3040,42 @@
         <v>81.859025799999998</v>
       </c>
       <c r="R13" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>605756.79091999994</v>
-      </c>
-      <c r="S13" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q12,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q12,"")</f>
         <v>43.529822599999996</v>
       </c>
+      <c r="S13" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>5.3351552199308028</v>
+      </c>
       <c r="T13" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>322120.68723999994</v>
-      </c>
-      <c r="U13" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>5.3351552199308028</v>
-      </c>
-      <c r="V13" s="5">
         <v>94.087449899999996</v>
       </c>
+      <c r="U13" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T12,"")</f>
+        <v>-9.0446457000000038</v>
+      </c>
+      <c r="V13" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>6.1321417468415902</v>
+      </c>
       <c r="W13" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>2145193.8577199997</v>
+        <v>13910.285795399999</v>
       </c>
       <c r="X13" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V12,"")</f>
-        <v>-9.0446457000000038</v>
-      </c>
-      <c r="Y13" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>-206217.92196000009</v>
-      </c>
-      <c r="Z13" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>6.1321417468415902</v>
-      </c>
-      <c r="AA13" s="5">
-        <v>13910.285795399999</v>
-      </c>
-      <c r="AB13" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA12,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W12,"")</f>
         <v>-16158.2027547</v>
       </c>
-      <c r="AC13" s="7">
+      <c r="Y13" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>906.6017234724726</v>
       </c>
-      <c r="AD13" s="6">
+      <c r="Z13" s="6">
         <v>15343326</v>
       </c>
+      <c r="AC13" s="3"/>
+      <c r="AD13" s="3"/>
+      <c r="AE13" s="3"/>
+      <c r="AF13" s="3"/>
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
       <c r="AI13" s="3"/>
@@ -3390,12 +3094,8 @@
       <c r="AV13" s="3"/>
       <c r="AW13" s="3"/>
       <c r="AX13" s="3"/>
-      <c r="AY13" s="3"/>
-      <c r="AZ13" s="3"/>
-      <c r="BA13" s="3"/>
-      <c r="BB13" s="3"/>
     </row>
-    <row r="14" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2001</v>
       </c>
@@ -3459,54 +3159,42 @@
         <v>155.34925490000001</v>
       </c>
       <c r="R14" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>1149584.4862600002</v>
-      </c>
-      <c r="S14" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q13,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q13,"")</f>
         <v>73.490229100000008</v>
       </c>
+      <c r="S14" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>10.009585337005056</v>
+      </c>
       <c r="T14" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>543827.69534000009</v>
-      </c>
-      <c r="U14" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>10.009585337005056</v>
-      </c>
-      <c r="V14" s="5">
         <v>98.643117899999993</v>
       </c>
+      <c r="U14" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T13,"")</f>
+        <v>4.5556679999999972</v>
+      </c>
+      <c r="V14" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>6.3558509319139391</v>
+      </c>
       <c r="W14" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>2249063.08812</v>
+        <v>10375.8785307</v>
       </c>
       <c r="X14" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V13,"")</f>
-        <v>4.5556679999999972</v>
-      </c>
-      <c r="Y14" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>103869.23039999994</v>
-      </c>
-      <c r="Z14" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>6.3558509319139391</v>
-      </c>
-      <c r="AA14" s="5">
-        <v>10375.8785307</v>
-      </c>
-      <c r="AB14" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA13,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W13,"")</f>
         <v>-3534.4072646999994</v>
       </c>
-      <c r="AC14" s="7">
+      <c r="Y14" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>668.54676365390333</v>
       </c>
-      <c r="AD14" s="6">
+      <c r="Z14" s="6">
         <v>15520049</v>
       </c>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
       <c r="AI14" s="3"/>
@@ -3525,12 +3213,8 @@
       <c r="AV14" s="3"/>
       <c r="AW14" s="3"/>
       <c r="AX14" s="3"/>
-      <c r="AY14" s="3"/>
-      <c r="AZ14" s="3"/>
-      <c r="BA14" s="3"/>
-      <c r="BB14" s="3"/>
     </row>
-    <row r="15" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>2002</v>
       </c>
@@ -3594,54 +3278,42 @@
         <v>190.21093819999999</v>
       </c>
       <c r="R15" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>1407560.9426799999</v>
-      </c>
-      <c r="S15" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q14,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q14,"")</f>
         <v>34.861683299999982</v>
       </c>
+      <c r="S15" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>12.121753925849083</v>
+      </c>
       <c r="T15" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>257976.45641999986</v>
-      </c>
-      <c r="U15" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>12.121753925849083</v>
-      </c>
-      <c r="V15" s="5">
         <v>96.009649400000001</v>
       </c>
+      <c r="U15" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T14,"")</f>
+        <v>-2.6334684999999922</v>
+      </c>
+      <c r="V15" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>6.1184985235188973</v>
+      </c>
       <c r="W15" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>2189020.0063200002</v>
+        <v>20475.969786199999</v>
       </c>
       <c r="X15" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V14,"")</f>
-        <v>-2.6334684999999922</v>
-      </c>
-      <c r="Y15" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>-60043.081799999825</v>
-      </c>
-      <c r="Z15" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>6.1184985235188973</v>
-      </c>
-      <c r="AA15" s="5">
-        <v>20475.969786199999</v>
-      </c>
-      <c r="AB15" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA14,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W14,"")</f>
         <v>10100.0912555</v>
       </c>
-      <c r="AC15" s="7">
+      <c r="Y15" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>1304.8916612800615</v>
       </c>
-      <c r="AD15" s="6">
+      <c r="Z15" s="6">
         <v>15691701</v>
       </c>
+      <c r="AC15" s="3"/>
+      <c r="AD15" s="3"/>
+      <c r="AE15" s="3"/>
+      <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
       <c r="AI15" s="3"/>
@@ -3660,12 +3332,8 @@
       <c r="AV15" s="3"/>
       <c r="AW15" s="3"/>
       <c r="AX15" s="3"/>
-      <c r="AY15" s="3"/>
-      <c r="AZ15" s="3"/>
-      <c r="BA15" s="3"/>
-      <c r="BB15" s="3"/>
     </row>
-    <row r="16" spans="1:60" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2003</v>
       </c>
@@ -3729,54 +3397,42 @@
         <v>209.97040569999999</v>
       </c>
       <c r="R16" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>1553781.0021799998</v>
-      </c>
-      <c r="S16" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q15,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q15,"")</f>
         <v>19.7594675</v>
       </c>
+      <c r="S16" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>13.241515435129912</v>
+      </c>
       <c r="T16" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>146220.0595</v>
-      </c>
-      <c r="U16" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>13.241515435129912</v>
-      </c>
-      <c r="V16" s="5">
         <v>136.45448529999999</v>
       </c>
+      <c r="U16" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T15,"")</f>
+        <v>40.444835899999987</v>
+      </c>
+      <c r="V16" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>8.6053278187891671</v>
+      </c>
       <c r="W16" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>3111162.2648399998</v>
+        <v>4022.6122099999998</v>
       </c>
       <c r="X16" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V15,"")</f>
-        <v>40.444835899999987</v>
-      </c>
-      <c r="Y16" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>922142.25851999968</v>
-      </c>
-      <c r="Z16" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>8.6053278187891671</v>
-      </c>
-      <c r="AA16" s="5">
-        <v>4022.6122099999998</v>
-      </c>
-      <c r="AB16" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA15,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W15,"")</f>
         <v>-16453.3575762</v>
       </c>
-      <c r="AC16" s="7">
+      <c r="Y16" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>253.68090084257545</v>
       </c>
-      <c r="AD16" s="6">
+      <c r="Z16" s="6">
         <v>15856977</v>
       </c>
+      <c r="AC16" s="3"/>
+      <c r="AD16" s="3"/>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
       <c r="AG16" s="3"/>
       <c r="AH16" s="3"/>
       <c r="AI16" s="3"/>
@@ -3795,12 +3451,8 @@
       <c r="AV16" s="3"/>
       <c r="AW16" s="3"/>
       <c r="AX16" s="3"/>
-      <c r="AY16" s="3"/>
-      <c r="AZ16" s="3"/>
-      <c r="BA16" s="3"/>
-      <c r="BB16" s="3"/>
     </row>
-    <row r="17" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>2004</v>
       </c>
@@ -3864,54 +3516,42 @@
         <v>245.87568210000001</v>
       </c>
       <c r="R17" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>1819480.0475399999</v>
-      </c>
-      <c r="S17" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q16,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q16,"")</f>
         <v>35.90527640000002</v>
       </c>
+      <c r="S17" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>15.346001815114132</v>
+      </c>
       <c r="T17" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>265699.04536000016</v>
-      </c>
-      <c r="U17" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>15.346001815114132</v>
-      </c>
-      <c r="V17" s="5">
         <v>122.5370099</v>
       </c>
+      <c r="U17" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T16,"")</f>
+        <v>-13.917475399999987</v>
+      </c>
+      <c r="V17" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>7.647983567481309</v>
+      </c>
       <c r="W17" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>2793843.8257200001</v>
+        <v>15742.7007526</v>
       </c>
       <c r="X17" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V16,"")</f>
-        <v>-13.917475399999987</v>
-      </c>
-      <c r="Y17" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>-317318.4391199997</v>
-      </c>
-      <c r="Z17" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>7.647983567481309</v>
-      </c>
-      <c r="AA17" s="5">
-        <v>15742.7007526</v>
-      </c>
-      <c r="AB17" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA16,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W16,"")</f>
         <v>11720.0885426</v>
       </c>
-      <c r="AC17" s="7">
+      <c r="Y17" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>982.55961004692688</v>
       </c>
-      <c r="AD17" s="6">
+      <c r="Z17" s="6">
         <v>16022133</v>
       </c>
+      <c r="AC17" s="3"/>
+      <c r="AD17" s="3"/>
+      <c r="AE17" s="3"/>
+      <c r="AF17" s="3"/>
       <c r="AG17" s="3"/>
       <c r="AH17" s="3"/>
       <c r="AI17" s="3"/>
@@ -3930,12 +3570,8 @@
       <c r="AV17" s="3"/>
       <c r="AW17" s="3"/>
       <c r="AX17" s="3"/>
-      <c r="AY17" s="3"/>
-      <c r="AZ17" s="3"/>
-      <c r="BA17" s="3"/>
-      <c r="BB17" s="3"/>
     </row>
-    <row r="18" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>2005</v>
       </c>
@@ -3999,54 +3635,42 @@
         <v>279.79542859999998</v>
       </c>
       <c r="R18" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>2070486.1716399998</v>
-      </c>
-      <c r="S18" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q17,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q17,"")</f>
         <v>33.919746499999974</v>
       </c>
+      <c r="S18" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>17.288943601716539</v>
+      </c>
       <c r="T18" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>251006.12409999981</v>
-      </c>
-      <c r="U18" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>17.288943601716539</v>
-      </c>
-      <c r="V18" s="5">
         <v>113.3410167</v>
       </c>
+      <c r="U18" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T17,"")</f>
+        <v>-9.1959932000000038</v>
+      </c>
+      <c r="V18" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>7.0034970024078245</v>
+      </c>
       <c r="W18" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>2584175.1807599999</v>
+        <v>18237.449836200001</v>
       </c>
       <c r="X18" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V17,"")</f>
-        <v>-9.1959932000000038</v>
-      </c>
-      <c r="Y18" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>-209668.64496000009</v>
-      </c>
-      <c r="Z18" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>7.0034970024078245</v>
-      </c>
-      <c r="AA18" s="5">
-        <v>18237.449836200001</v>
-      </c>
-      <c r="AB18" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA17,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W17,"")</f>
         <v>2494.7490836000015</v>
       </c>
-      <c r="AC18" s="7">
+      <c r="Y18" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>1126.9170594919303</v>
       </c>
-      <c r="AD18" s="6">
+      <c r="Z18" s="6">
         <v>16183489</v>
       </c>
+      <c r="AC18" s="3"/>
+      <c r="AD18" s="3"/>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
       <c r="AI18" s="3"/>
@@ -4065,12 +3689,8 @@
       <c r="AV18" s="3"/>
       <c r="AW18" s="3"/>
       <c r="AX18" s="3"/>
-      <c r="AY18" s="3"/>
-      <c r="AZ18" s="3"/>
-      <c r="BA18" s="3"/>
-      <c r="BB18" s="3"/>
     </row>
-    <row r="19" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>2006</v>
       </c>
@@ -4134,54 +3754,42 @@
         <v>380.26127020000001</v>
       </c>
       <c r="R19" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>2813933.3994800001</v>
-      </c>
-      <c r="S19" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q18,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q18,"")</f>
         <v>100.46584160000003</v>
       </c>
+      <c r="S19" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>23.260571865849354</v>
+      </c>
       <c r="T19" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>743447.2278400003</v>
-      </c>
-      <c r="U19" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>23.260571865849354</v>
-      </c>
-      <c r="V19" s="5">
         <v>129.73571219999999</v>
       </c>
+      <c r="U19" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T18,"")</f>
+        <v>16.394695499999997</v>
+      </c>
+      <c r="V19" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>7.9359300925073519</v>
+      </c>
       <c r="W19" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>2957974.2381599997</v>
+        <v>15633.587788299999</v>
       </c>
       <c r="X19" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V18,"")</f>
-        <v>16.394695499999997</v>
-      </c>
-      <c r="Y19" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>373799.05739999993</v>
-      </c>
-      <c r="Z19" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>7.9359300925073519</v>
-      </c>
-      <c r="AA19" s="5">
-        <v>15633.587788299999</v>
-      </c>
-      <c r="AB19" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA18,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W18,"")</f>
         <v>-2603.8620479000019</v>
       </c>
-      <c r="AC19" s="7">
+      <c r="Y19" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>956.30615255546741</v>
       </c>
-      <c r="AD19" s="6">
+      <c r="Z19" s="6">
         <v>16347890</v>
       </c>
+      <c r="AC19" s="3"/>
+      <c r="AD19" s="3"/>
+      <c r="AE19" s="3"/>
+      <c r="AF19" s="3"/>
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
       <c r="AI19" s="3"/>
@@ -4200,12 +3808,8 @@
       <c r="AV19" s="3"/>
       <c r="AW19" s="3"/>
       <c r="AX19" s="3"/>
-      <c r="AY19" s="3"/>
-      <c r="AZ19" s="3"/>
-      <c r="BA19" s="3"/>
-      <c r="BB19" s="3"/>
     </row>
-    <row r="20" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>2007</v>
       </c>
@@ -4269,54 +3873,42 @@
         <v>482.06876949999997</v>
       </c>
       <c r="R20" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>3567308.8942999998</v>
-      </c>
-      <c r="S20" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q19,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q19,"")</f>
         <v>101.80749929999996</v>
       </c>
+      <c r="S20" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>29.184569855078113</v>
+      </c>
       <c r="T20" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>753375.49481999967</v>
-      </c>
-      <c r="U20" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>29.184569855078113</v>
-      </c>
-      <c r="V20" s="5">
         <v>145.21709680000001</v>
       </c>
+      <c r="U20" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T19,"")</f>
+        <v>15.481384600000013</v>
+      </c>
+      <c r="V20" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>8.7914811617167832</v>
+      </c>
       <c r="W20" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>3310949.8070400003</v>
+        <v>37560.526304200001</v>
       </c>
       <c r="X20" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V19,"")</f>
-        <v>15.481384600000013</v>
-      </c>
-      <c r="Y20" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>352975.56888000027</v>
-      </c>
-      <c r="Z20" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>8.7914811617167832</v>
-      </c>
-      <c r="AA20" s="5">
-        <v>37560.526304200001</v>
-      </c>
-      <c r="AB20" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA19,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W19,"")</f>
         <v>21926.938515900001</v>
       </c>
-      <c r="AC20" s="7">
+      <c r="Y20" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>2273.9241226005702</v>
       </c>
-      <c r="AD20" s="6">
+      <c r="Z20" s="6">
         <v>16517933</v>
       </c>
+      <c r="AC20" s="3"/>
+      <c r="AD20" s="3"/>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
       <c r="AI20" s="3"/>
@@ -4335,12 +3927,8 @@
       <c r="AV20" s="3"/>
       <c r="AW20" s="3"/>
       <c r="AX20" s="3"/>
-      <c r="AY20" s="3"/>
-      <c r="AZ20" s="3"/>
-      <c r="BA20" s="3"/>
-      <c r="BB20" s="3"/>
     </row>
-    <row r="21" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>2008</v>
       </c>
@@ -4404,54 +3992,42 @@
         <v>643.54795379999996</v>
       </c>
       <c r="R21" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>4762254.85812</v>
-      </c>
-      <c r="S21" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q20,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q20,"")</f>
         <v>161.47918429999999</v>
       </c>
+      <c r="S21" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>38.540989033614935</v>
+      </c>
       <c r="T21" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>1194945.9638199999</v>
-      </c>
-      <c r="U21" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>38.540989033614935</v>
-      </c>
-      <c r="V21" s="5">
         <v>178.86223150000001</v>
       </c>
+      <c r="U21" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T20,"")</f>
+        <v>33.6451347</v>
+      </c>
+      <c r="V21" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>10.711753898158998</v>
+      </c>
       <c r="W21" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>4078058.8782000002</v>
+        <v>36250.329240699997</v>
       </c>
       <c r="X21" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V20,"")</f>
-        <v>33.6451347</v>
-      </c>
-      <c r="Y21" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>767109.07116000005</v>
-      </c>
-      <c r="Z21" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>10.711753898158998</v>
-      </c>
-      <c r="AA21" s="5">
-        <v>36250.329240699997</v>
-      </c>
-      <c r="AB21" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA20,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W20,"")</f>
         <v>-1310.1970635000034</v>
       </c>
-      <c r="AC21" s="7">
+      <c r="Y21" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>2170.97037366223</v>
       </c>
-      <c r="AD21" s="6">
+      <c r="Z21" s="6">
         <v>16697754</v>
       </c>
+      <c r="AC21" s="3"/>
+      <c r="AD21" s="3"/>
+      <c r="AE21" s="3"/>
+      <c r="AF21" s="3"/>
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
       <c r="AI21" s="3"/>
@@ -4470,12 +4046,8 @@
       <c r="AV21" s="3"/>
       <c r="AW21" s="3"/>
       <c r="AX21" s="3"/>
-      <c r="AY21" s="3"/>
-      <c r="AZ21" s="3"/>
-      <c r="BA21" s="3"/>
-      <c r="BB21" s="3"/>
     </row>
-    <row r="22" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>2009</v>
       </c>
@@ -4539,54 +4111,42 @@
         <v>757.469784</v>
       </c>
       <c r="R22" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>5605276.4016000004</v>
-      </c>
-      <c r="S22" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q21,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q21,"")</f>
         <v>113.92183020000004</v>
       </c>
+      <c r="S22" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>44.870936796808827</v>
+      </c>
       <c r="T22" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>843021.54348000034</v>
-      </c>
-      <c r="U22" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>44.870936796808827</v>
-      </c>
-      <c r="V22" s="5">
         <v>168.69801240000001</v>
       </c>
+      <c r="U22" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T21,"")</f>
+        <v>-10.164219099999997</v>
+      </c>
+      <c r="V22" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>9.9933198815857622</v>
+      </c>
       <c r="W22" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>3846314.6827200004</v>
+        <v>28351.725175600001</v>
       </c>
       <c r="X22" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V21,"")</f>
-        <v>-10.164219099999997</v>
-      </c>
-      <c r="Y22" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>-231744.19547999994</v>
-      </c>
-      <c r="Z22" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>9.9933198815857622</v>
-      </c>
-      <c r="AA22" s="5">
-        <v>28351.725175600001</v>
-      </c>
-      <c r="AB22" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA21,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W21,"")</f>
         <v>-7898.6040650999967</v>
       </c>
-      <c r="AC22" s="7">
+      <c r="Y22" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>1679.4973150174415</v>
       </c>
-      <c r="AD22" s="6">
+      <c r="Z22" s="6">
         <v>16881078</v>
       </c>
+      <c r="AC22" s="3"/>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
       <c r="AG22" s="3"/>
       <c r="AH22" s="3"/>
       <c r="AI22" s="3"/>
@@ -4605,12 +4165,8 @@
       <c r="AV22" s="3"/>
       <c r="AW22" s="3"/>
       <c r="AX22" s="3"/>
-      <c r="AY22" s="3"/>
-      <c r="AZ22" s="3"/>
-      <c r="BA22" s="3"/>
-      <c r="BB22" s="3"/>
     </row>
-    <row r="23" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>2010</v>
       </c>
@@ -4674,54 +4230,42 @@
         <v>1000.072309</v>
       </c>
       <c r="R23" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>7400535.0866</v>
-      </c>
-      <c r="S23" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q22,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q22,"")</f>
         <v>242.60252500000001</v>
       </c>
+      <c r="S23" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>58.607394944903362</v>
+      </c>
       <c r="T23" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>1795258.6850000001</v>
-      </c>
-      <c r="U23" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>58.607394944903362</v>
-      </c>
-      <c r="V23" s="5">
         <v>242.69112910000001</v>
       </c>
+      <c r="U23" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T22,"")</f>
+        <v>73.993116700000002</v>
+      </c>
+      <c r="V23" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>14.222466440462386</v>
+      </c>
       <c r="W23" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>5533357.7434800006</v>
+        <v>19931.373417300001</v>
       </c>
       <c r="X23" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V22,"")</f>
-        <v>73.993116700000002</v>
-      </c>
-      <c r="Y23" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>1687043.06076</v>
-      </c>
-      <c r="Z23" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>14.222466440462386</v>
-      </c>
-      <c r="AA23" s="5">
-        <v>19931.373417300001</v>
-      </c>
-      <c r="AB23" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA22,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W22,"")</f>
         <v>-8420.3517582999993</v>
       </c>
-      <c r="AC23" s="7">
+      <c r="Y23" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>1168.0414137554621</v>
       </c>
-      <c r="AD23" s="6">
+      <c r="Z23" s="6">
         <v>17063927</v>
       </c>
+      <c r="AC23" s="3"/>
+      <c r="AD23" s="3"/>
+      <c r="AE23" s="3"/>
+      <c r="AF23" s="3"/>
       <c r="AG23" s="3"/>
       <c r="AH23" s="3"/>
       <c r="AI23" s="3"/>
@@ -4740,12 +4284,8 @@
       <c r="AV23" s="3"/>
       <c r="AW23" s="3"/>
       <c r="AX23" s="3"/>
-      <c r="AY23" s="3"/>
-      <c r="AZ23" s="3"/>
-      <c r="BA23" s="3"/>
-      <c r="BB23" s="3"/>
     </row>
-    <row r="24" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>2011</v>
       </c>
@@ -4809,54 +4349,42 @@
         <v>1318.1949703</v>
       </c>
       <c r="R24" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>9754642.7802200001</v>
-      </c>
-      <c r="S24" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q23,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q23,"")</f>
         <v>318.1226613</v>
       </c>
+      <c r="S24" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>76.398679895090794</v>
+      </c>
       <c r="T24" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>2354107.69362</v>
-      </c>
-      <c r="U24" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>76.398679895090794</v>
-      </c>
-      <c r="V24" s="5">
         <v>244.8478355</v>
       </c>
+      <c r="U24" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T23,"")</f>
+        <v>2.1567063999999903</v>
+      </c>
+      <c r="V24" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>14.190656032554239</v>
+      </c>
       <c r="W24" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>5582530.6494000005</v>
+        <v>34345.134085600002</v>
       </c>
       <c r="X24" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V23,"")</f>
-        <v>2.1567063999999903</v>
-      </c>
-      <c r="Y24" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>49172.905919999779</v>
-      </c>
-      <c r="Z24" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>14.190656032554239</v>
-      </c>
-      <c r="AA24" s="5">
-        <v>34345.134085600002</v>
-      </c>
-      <c r="AB24" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA23,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W23,"")</f>
         <v>14413.760668300001</v>
       </c>
-      <c r="AC24" s="7">
+      <c r="Y24" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>1990.5423431880974</v>
       </c>
-      <c r="AD24" s="6">
+      <c r="Z24" s="6">
         <v>17254159</v>
       </c>
+      <c r="AC24" s="3"/>
+      <c r="AD24" s="3"/>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
       <c r="AG24" s="3"/>
       <c r="AH24" s="3"/>
       <c r="AI24" s="3"/>
@@ -4875,12 +4403,8 @@
       <c r="AV24" s="3"/>
       <c r="AW24" s="3"/>
       <c r="AX24" s="3"/>
-      <c r="AY24" s="3"/>
-      <c r="AZ24" s="3"/>
-      <c r="BA24" s="3"/>
-      <c r="BB24" s="3"/>
     </row>
-    <row r="25" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>2012</v>
       </c>
@@ -4944,54 +4468,42 @@
         <v>1582.9674031</v>
       </c>
       <c r="R25" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>11713958.78294</v>
-      </c>
-      <c r="S25" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q24,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q24,"")</f>
         <v>264.77243279999993</v>
       </c>
+      <c r="S25" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>90.748314262322836</v>
+      </c>
       <c r="T25" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>1959316.0027199995</v>
-      </c>
-      <c r="U25" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>90.748314262322836</v>
-      </c>
-      <c r="V25" s="5">
         <v>233.0762191</v>
       </c>
+      <c r="U25" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T24,"")</f>
+        <v>-11.771616399999999</v>
+      </c>
+      <c r="V25" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>13.361787448395507</v>
+      </c>
       <c r="W25" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>5314137.7954799999</v>
+        <v>43061.174613700001</v>
       </c>
       <c r="X25" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V24,"")</f>
-        <v>-11.771616399999999</v>
-      </c>
-      <c r="Y25" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>-268392.85391999997</v>
-      </c>
-      <c r="Z25" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>13.361787448395507</v>
-      </c>
-      <c r="AA25" s="5">
-        <v>43061.174613700001</v>
-      </c>
-      <c r="AB25" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA24,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W24,"")</f>
         <v>8716.0405280999985</v>
       </c>
-      <c r="AC25" s="7">
+      <c r="Y25" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>2468.6099023240245</v>
       </c>
-      <c r="AD25" s="6">
+      <c r="Z25" s="6">
         <v>17443491</v>
       </c>
+      <c r="AC25" s="3"/>
+      <c r="AD25" s="3"/>
+      <c r="AE25" s="3"/>
+      <c r="AF25" s="3"/>
       <c r="AG25" s="3"/>
       <c r="AH25" s="3"/>
       <c r="AI25" s="3"/>
@@ -5010,12 +4522,8 @@
       <c r="AV25" s="3"/>
       <c r="AW25" s="3"/>
       <c r="AX25" s="3"/>
-      <c r="AY25" s="3"/>
-      <c r="AZ25" s="3"/>
-      <c r="BA25" s="3"/>
-      <c r="BB25" s="3"/>
     </row>
-    <row r="26" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>2013</v>
       </c>
@@ -5079,54 +4587,42 @@
         <v>1868.1165939</v>
       </c>
       <c r="R26" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>13824062.79486</v>
-      </c>
-      <c r="S26" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q25,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q25,"")</f>
         <v>285.14919080000004</v>
       </c>
+      <c r="S26" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>106.0712576018195</v>
+      </c>
       <c r="T26" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>2110104.0119200004</v>
-      </c>
-      <c r="U26" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>106.0712576018195</v>
-      </c>
-      <c r="V26" s="5">
         <v>233.82480039999999</v>
       </c>
+      <c r="U26" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T25,"")</f>
+        <v>0.74858129999998368</v>
+      </c>
+      <c r="V26" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>13.276521774877011</v>
+      </c>
       <c r="W26" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>5331205.44912</v>
+        <v>32416.8563975</v>
       </c>
       <c r="X26" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V25,"")</f>
-        <v>0.74858129999998368</v>
-      </c>
-      <c r="Y26" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>17067.653639999629</v>
-      </c>
-      <c r="Z26" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>13.276521774877011</v>
-      </c>
-      <c r="AA26" s="5">
-        <v>32416.8563975</v>
-      </c>
-      <c r="AB26" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA25,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W25,"")</f>
         <v>-10644.318216200001</v>
       </c>
-      <c r="AC26" s="7">
+      <c r="Y26" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>1840.6221200583559</v>
       </c>
-      <c r="AD26" s="6">
+      <c r="Z26" s="6">
         <v>17611902</v>
       </c>
+      <c r="AC26" s="3"/>
+      <c r="AD26" s="3"/>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
       <c r="AG26" s="3"/>
       <c r="AH26" s="3"/>
       <c r="AI26" s="3"/>
@@ -5145,12 +4641,8 @@
       <c r="AV26" s="3"/>
       <c r="AW26" s="3"/>
       <c r="AX26" s="3"/>
-      <c r="AY26" s="3"/>
-      <c r="AZ26" s="3"/>
-      <c r="BA26" s="3"/>
-      <c r="BB26" s="3"/>
     </row>
-    <row r="27" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>2014</v>
       </c>
@@ -5214,54 +4706,42 @@
         <v>2337.3739160999999</v>
       </c>
       <c r="R27" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>17296566.979139999</v>
-      </c>
-      <c r="S27" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q26,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q26,"")</f>
         <v>469.25732219999986</v>
       </c>
+      <c r="S27" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>131.40455610776868</v>
+      </c>
       <c r="T27" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>3472504.1842799988</v>
-      </c>
-      <c r="U27" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>131.40455610776868</v>
-      </c>
-      <c r="V27" s="5">
         <v>232.89751129999999</v>
       </c>
+      <c r="U27" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T26,"")</f>
+        <v>-0.92728909999999587</v>
+      </c>
+      <c r="V27" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>13.09323847595774</v>
+      </c>
       <c r="W27" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>5310063.2576399995</v>
+        <v>45751.527614400002</v>
       </c>
       <c r="X27" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V26,"")</f>
-        <v>-0.92728909999999587</v>
-      </c>
-      <c r="Y27" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>-21142.191479999907</v>
-      </c>
-      <c r="Z27" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>13.09323847595774</v>
-      </c>
-      <c r="AA27" s="5">
-        <v>45751.527614400002</v>
-      </c>
-      <c r="AB27" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA26,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W26,"")</f>
         <v>13334.671216900002</v>
       </c>
-      <c r="AC27" s="7">
+      <c r="Y27" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>2572.099883553823</v>
       </c>
-      <c r="AD27" s="6">
+      <c r="Z27" s="6">
         <v>17787617</v>
       </c>
+      <c r="AC27" s="3"/>
+      <c r="AD27" s="3"/>
+      <c r="AE27" s="3"/>
+      <c r="AF27" s="3"/>
       <c r="AG27" s="3"/>
       <c r="AH27" s="3"/>
       <c r="AI27" s="3"/>
@@ -5280,12 +4760,8 @@
       <c r="AV27" s="3"/>
       <c r="AW27" s="3"/>
       <c r="AX27" s="3"/>
-      <c r="AY27" s="3"/>
-      <c r="AZ27" s="3"/>
-      <c r="BA27" s="3"/>
-      <c r="BB27" s="3"/>
     </row>
-    <row r="28" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>2015</v>
       </c>
@@ -5349,54 +4825,42 @@
         <v>2588.7588488000001</v>
       </c>
       <c r="R28" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>19156815.481120002</v>
-      </c>
-      <c r="S28" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q27,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q27,"")</f>
         <v>251.38493270000026</v>
       </c>
+      <c r="S28" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>144.04862924878014</v>
+      </c>
       <c r="T28" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>1860248.501980002</v>
-      </c>
-      <c r="U28" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>144.04862924878014</v>
-      </c>
-      <c r="V28" s="5">
         <v>242.32577929999999</v>
       </c>
+      <c r="U28" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T27,"")</f>
+        <v>9.4282680000000028</v>
+      </c>
+      <c r="V28" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>13.483950564181812</v>
+      </c>
       <c r="W28" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>5525027.7680399995</v>
+        <v>63270.943081500001</v>
       </c>
       <c r="X28" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V27,"")</f>
-        <v>9.4282680000000028</v>
-      </c>
-      <c r="Y28" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>214964.51040000006</v>
-      </c>
-      <c r="Z28" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>13.483950564181812</v>
-      </c>
-      <c r="AA28" s="5">
-        <v>63270.943081500001</v>
-      </c>
-      <c r="AB28" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA27,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W27,"")</f>
         <v>17519.4154671</v>
       </c>
-      <c r="AC28" s="7">
+      <c r="Y28" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>3520.6418034620856</v>
       </c>
-      <c r="AD28" s="6">
+      <c r="Z28" s="6">
         <v>17971423</v>
       </c>
+      <c r="AC28" s="3"/>
+      <c r="AD28" s="3"/>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
       <c r="AG28" s="3"/>
       <c r="AH28" s="3"/>
       <c r="AI28" s="3"/>
@@ -5415,12 +4879,8 @@
       <c r="AV28" s="3"/>
       <c r="AW28" s="3"/>
       <c r="AX28" s="3"/>
-      <c r="AY28" s="3"/>
-      <c r="AZ28" s="3"/>
-      <c r="BA28" s="3"/>
-      <c r="BB28" s="3"/>
     </row>
-    <row r="29" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:50" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>2016</v>
       </c>
@@ -5484,54 +4944,42 @@
         <v>2869.4604433</v>
       </c>
       <c r="R29" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[HFC]]*7400</f>
-        <v>21234007.280419998</v>
-      </c>
-      <c r="S29" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC]]-Q28,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]-Q28,"")</f>
         <v>280.70159449999983</v>
       </c>
+      <c r="S29" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[HFC (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>157.94777481021097</v>
+      </c>
       <c r="T29" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación HFC]]*7400</f>
-        <v>2077191.7992999987</v>
-      </c>
-      <c r="U29" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[HFC]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>157.94777481021097</v>
-      </c>
-      <c r="V29" s="5">
         <v>272.26847249999997</v>
       </c>
+      <c r="U29" s="5">
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]-T28,"")</f>
+        <v>29.942693199999979</v>
+      </c>
+      <c r="V29" s="7">
+        <f>(Todo_Gases_Chile[[#This Row],[SF6 (CO2eq)]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
+        <v>14.986859108917871</v>
+      </c>
       <c r="W29" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[SF6]]*22800</f>
-        <v>6207721.1729999995</v>
+        <v>46185.174907799999</v>
       </c>
       <c r="X29" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[SF6]]-V28,"")</f>
-        <v>29.942693199999979</v>
-      </c>
-      <c r="Y29" s="5">
-        <f>Todo_Gases_Chile[[#This Row],[Variación SF6]]*22800</f>
-        <v>682693.40495999949</v>
-      </c>
-      <c r="Z29" s="7">
-        <f>(Todo_Gases_Chile[[#This Row],[SF6]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
-        <v>14.986859108917871</v>
-      </c>
-      <c r="AA29" s="5">
-        <v>46185.174907799999</v>
-      </c>
-      <c r="AB29" s="5">
-        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-AA28,"")</f>
+        <f>IFERROR(Todo_Gases_Chile[[#This Row],[CO2eq]]-W28,"")</f>
         <v>-17085.768173700002</v>
       </c>
-      <c r="AC29" s="7">
+      <c r="Y29" s="7">
         <f>(Todo_Gases_Chile[[#This Row],[CO2eq]]/Todo_Gases_Chile[[#This Row],[Población]])*1000000</f>
         <v>2542.2359882814844</v>
       </c>
-      <c r="AD29" s="6">
+      <c r="Z29" s="6">
         <v>18167147</v>
       </c>
+      <c r="AC29" s="3"/>
+      <c r="AD29" s="3"/>
+      <c r="AE29" s="3"/>
+      <c r="AF29" s="3"/>
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
       <c r="AI29" s="3"/>
@@ -5550,12 +4998,12 @@
       <c r="AV29" s="3"/>
       <c r="AW29" s="3"/>
       <c r="AX29" s="3"/>
-      <c r="AY29" s="3"/>
-      <c r="AZ29" s="3"/>
-      <c r="BA29" s="3"/>
-      <c r="BB29" s="3"/>
     </row>
-    <row r="30" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AC30" s="3"/>
+      <c r="AD30" s="3"/>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
       <c r="AG30" s="3"/>
       <c r="AH30" s="3"/>
       <c r="AI30" s="3"/>
@@ -5574,12 +5022,12 @@
       <c r="AV30" s="3"/>
       <c r="AW30" s="3"/>
       <c r="AX30" s="3"/>
-      <c r="AY30" s="3"/>
-      <c r="AZ30" s="3"/>
-      <c r="BA30" s="3"/>
-      <c r="BB30" s="3"/>
     </row>
-    <row r="31" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AC31" s="3"/>
+      <c r="AD31" s="3"/>
+      <c r="AE31" s="3"/>
+      <c r="AF31" s="3"/>
       <c r="AG31" s="3"/>
       <c r="AH31" s="3"/>
       <c r="AI31" s="3"/>
@@ -5598,12 +5046,12 @@
       <c r="AV31" s="3"/>
       <c r="AW31" s="3"/>
       <c r="AX31" s="3"/>
-      <c r="AY31" s="3"/>
-      <c r="AZ31" s="3"/>
-      <c r="BA31" s="3"/>
-      <c r="BB31" s="3"/>
     </row>
-    <row r="32" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:50" x14ac:dyDescent="0.25">
+      <c r="AC32" s="3"/>
+      <c r="AD32" s="3"/>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
       <c r="AG32" s="3"/>
       <c r="AH32" s="3"/>
       <c r="AI32" s="3"/>
@@ -5622,12 +5070,12 @@
       <c r="AV32" s="3"/>
       <c r="AW32" s="3"/>
       <c r="AX32" s="3"/>
-      <c r="AY32" s="3"/>
-      <c r="AZ32" s="3"/>
-      <c r="BA32" s="3"/>
-      <c r="BB32" s="3"/>
     </row>
-    <row r="33" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="33" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC33" s="3"/>
+      <c r="AD33" s="3"/>
+      <c r="AE33" s="3"/>
+      <c r="AF33" s="3"/>
       <c r="AG33" s="3"/>
       <c r="AH33" s="3"/>
       <c r="AI33" s="3"/>
@@ -5646,12 +5094,12 @@
       <c r="AV33" s="3"/>
       <c r="AW33" s="3"/>
       <c r="AX33" s="3"/>
-      <c r="AY33" s="3"/>
-      <c r="AZ33" s="3"/>
-      <c r="BA33" s="3"/>
-      <c r="BB33" s="3"/>
     </row>
-    <row r="34" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="34" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC34" s="3"/>
+      <c r="AD34" s="3"/>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="3"/>
       <c r="AG34" s="3"/>
       <c r="AH34" s="3"/>
       <c r="AI34" s="3"/>
@@ -5670,12 +5118,12 @@
       <c r="AV34" s="3"/>
       <c r="AW34" s="3"/>
       <c r="AX34" s="3"/>
-      <c r="AY34" s="3"/>
-      <c r="AZ34" s="3"/>
-      <c r="BA34" s="3"/>
-      <c r="BB34" s="3"/>
     </row>
-    <row r="35" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="35" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC35" s="3"/>
+      <c r="AD35" s="3"/>
+      <c r="AE35" s="3"/>
+      <c r="AF35" s="3"/>
       <c r="AG35" s="3"/>
       <c r="AH35" s="3"/>
       <c r="AI35" s="3"/>
@@ -5694,12 +5142,12 @@
       <c r="AV35" s="3"/>
       <c r="AW35" s="3"/>
       <c r="AX35" s="3"/>
-      <c r="AY35" s="3"/>
-      <c r="AZ35" s="3"/>
-      <c r="BA35" s="3"/>
-      <c r="BB35" s="3"/>
     </row>
-    <row r="36" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="36" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC36" s="3"/>
+      <c r="AD36" s="3"/>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3"/>
       <c r="AG36" s="3"/>
       <c r="AH36" s="3"/>
       <c r="AI36" s="3"/>
@@ -5718,12 +5166,12 @@
       <c r="AV36" s="3"/>
       <c r="AW36" s="3"/>
       <c r="AX36" s="3"/>
-      <c r="AY36" s="3"/>
-      <c r="AZ36" s="3"/>
-      <c r="BA36" s="3"/>
-      <c r="BB36" s="3"/>
     </row>
-    <row r="37" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="37" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC37" s="3"/>
+      <c r="AD37" s="3"/>
+      <c r="AE37" s="3"/>
+      <c r="AF37" s="3"/>
       <c r="AG37" s="3"/>
       <c r="AH37" s="3"/>
       <c r="AI37" s="3"/>
@@ -5742,12 +5190,12 @@
       <c r="AV37" s="3"/>
       <c r="AW37" s="3"/>
       <c r="AX37" s="3"/>
-      <c r="AY37" s="3"/>
-      <c r="AZ37" s="3"/>
-      <c r="BA37" s="3"/>
-      <c r="BB37" s="3"/>
     </row>
-    <row r="38" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="38" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC38" s="3"/>
+      <c r="AD38" s="3"/>
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="3"/>
       <c r="AG38" s="3"/>
       <c r="AH38" s="3"/>
       <c r="AI38" s="3"/>
@@ -5766,12 +5214,12 @@
       <c r="AV38" s="3"/>
       <c r="AW38" s="3"/>
       <c r="AX38" s="3"/>
-      <c r="AY38" s="3"/>
-      <c r="AZ38" s="3"/>
-      <c r="BA38" s="3"/>
-      <c r="BB38" s="3"/>
     </row>
-    <row r="39" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="39" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC39" s="3"/>
+      <c r="AD39" s="3"/>
+      <c r="AE39" s="3"/>
+      <c r="AF39" s="3"/>
       <c r="AG39" s="3"/>
       <c r="AH39" s="3"/>
       <c r="AI39" s="3"/>
@@ -5790,12 +5238,12 @@
       <c r="AV39" s="3"/>
       <c r="AW39" s="3"/>
       <c r="AX39" s="3"/>
-      <c r="AY39" s="3"/>
-      <c r="AZ39" s="3"/>
-      <c r="BA39" s="3"/>
-      <c r="BB39" s="3"/>
     </row>
-    <row r="40" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="40" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC40" s="3"/>
+      <c r="AD40" s="3"/>
+      <c r="AE40" s="3"/>
+      <c r="AF40" s="3"/>
       <c r="AG40" s="3"/>
       <c r="AH40" s="3"/>
       <c r="AI40" s="3"/>
@@ -5814,12 +5262,12 @@
       <c r="AV40" s="3"/>
       <c r="AW40" s="3"/>
       <c r="AX40" s="3"/>
-      <c r="AY40" s="3"/>
-      <c r="AZ40" s="3"/>
-      <c r="BA40" s="3"/>
-      <c r="BB40" s="3"/>
     </row>
-    <row r="41" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="41" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC41" s="3"/>
+      <c r="AD41" s="3"/>
+      <c r="AE41" s="3"/>
+      <c r="AF41" s="3"/>
       <c r="AG41" s="3"/>
       <c r="AH41" s="3"/>
       <c r="AI41" s="3"/>
@@ -5838,12 +5286,12 @@
       <c r="AV41" s="3"/>
       <c r="AW41" s="3"/>
       <c r="AX41" s="3"/>
-      <c r="AY41" s="3"/>
-      <c r="AZ41" s="3"/>
-      <c r="BA41" s="3"/>
-      <c r="BB41" s="3"/>
     </row>
-    <row r="42" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="42" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC42" s="3"/>
+      <c r="AD42" s="3"/>
+      <c r="AE42" s="3"/>
+      <c r="AF42" s="3"/>
       <c r="AG42" s="3"/>
       <c r="AH42" s="3"/>
       <c r="AI42" s="3"/>
@@ -5862,12 +5310,12 @@
       <c r="AV42" s="3"/>
       <c r="AW42" s="3"/>
       <c r="AX42" s="3"/>
-      <c r="AY42" s="3"/>
-      <c r="AZ42" s="3"/>
-      <c r="BA42" s="3"/>
-      <c r="BB42" s="3"/>
     </row>
-    <row r="43" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="43" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC43" s="3"/>
+      <c r="AD43" s="3"/>
+      <c r="AE43" s="3"/>
+      <c r="AF43" s="3"/>
       <c r="AG43" s="3"/>
       <c r="AH43" s="3"/>
       <c r="AI43" s="3"/>
@@ -5886,12 +5334,12 @@
       <c r="AV43" s="3"/>
       <c r="AW43" s="3"/>
       <c r="AX43" s="3"/>
-      <c r="AY43" s="3"/>
-      <c r="AZ43" s="3"/>
-      <c r="BA43" s="3"/>
-      <c r="BB43" s="3"/>
     </row>
-    <row r="44" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="44" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC44" s="3"/>
+      <c r="AD44" s="3"/>
+      <c r="AE44" s="3"/>
+      <c r="AF44" s="3"/>
       <c r="AG44" s="3"/>
       <c r="AH44" s="3"/>
       <c r="AI44" s="3"/>
@@ -5910,12 +5358,12 @@
       <c r="AV44" s="3"/>
       <c r="AW44" s="3"/>
       <c r="AX44" s="3"/>
-      <c r="AY44" s="3"/>
-      <c r="AZ44" s="3"/>
-      <c r="BA44" s="3"/>
-      <c r="BB44" s="3"/>
     </row>
-    <row r="45" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="45" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC45" s="3"/>
+      <c r="AD45" s="3"/>
+      <c r="AE45" s="3"/>
+      <c r="AF45" s="3"/>
       <c r="AG45" s="3"/>
       <c r="AH45" s="3"/>
       <c r="AI45" s="3"/>
@@ -5934,12 +5382,12 @@
       <c r="AV45" s="3"/>
       <c r="AW45" s="3"/>
       <c r="AX45" s="3"/>
-      <c r="AY45" s="3"/>
-      <c r="AZ45" s="3"/>
-      <c r="BA45" s="3"/>
-      <c r="BB45" s="3"/>
     </row>
-    <row r="46" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="46" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC46" s="3"/>
+      <c r="AD46" s="3"/>
+      <c r="AE46" s="3"/>
+      <c r="AF46" s="3"/>
       <c r="AG46" s="3"/>
       <c r="AH46" s="3"/>
       <c r="AI46" s="3"/>
@@ -5958,12 +5406,12 @@
       <c r="AV46" s="3"/>
       <c r="AW46" s="3"/>
       <c r="AX46" s="3"/>
-      <c r="AY46" s="3"/>
-      <c r="AZ46" s="3"/>
-      <c r="BA46" s="3"/>
-      <c r="BB46" s="3"/>
     </row>
-    <row r="47" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="47" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC47" s="3"/>
+      <c r="AD47" s="3"/>
+      <c r="AE47" s="3"/>
+      <c r="AF47" s="3"/>
       <c r="AG47" s="3"/>
       <c r="AH47" s="3"/>
       <c r="AI47" s="3"/>
@@ -5982,12 +5430,12 @@
       <c r="AV47" s="3"/>
       <c r="AW47" s="3"/>
       <c r="AX47" s="3"/>
-      <c r="AY47" s="3"/>
-      <c r="AZ47" s="3"/>
-      <c r="BA47" s="3"/>
-      <c r="BB47" s="3"/>
     </row>
-    <row r="48" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="48" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC48" s="3"/>
+      <c r="AD48" s="3"/>
+      <c r="AE48" s="3"/>
+      <c r="AF48" s="3"/>
       <c r="AG48" s="3"/>
       <c r="AH48" s="3"/>
       <c r="AI48" s="3"/>
@@ -6006,12 +5454,12 @@
       <c r="AV48" s="3"/>
       <c r="AW48" s="3"/>
       <c r="AX48" s="3"/>
-      <c r="AY48" s="3"/>
-      <c r="AZ48" s="3"/>
-      <c r="BA48" s="3"/>
-      <c r="BB48" s="3"/>
     </row>
-    <row r="49" spans="33:54" x14ac:dyDescent="0.25">
+    <row r="49" spans="29:50" x14ac:dyDescent="0.25">
+      <c r="AC49" s="3"/>
+      <c r="AD49" s="3"/>
+      <c r="AE49" s="3"/>
+      <c r="AF49" s="3"/>
       <c r="AG49" s="3"/>
       <c r="AH49" s="3"/>
       <c r="AI49" s="3"/>
@@ -6030,14 +5478,10 @@
       <c r="AV49" s="3"/>
       <c r="AW49" s="3"/>
       <c r="AX49" s="3"/>
-      <c r="AY49" s="3"/>
-      <c r="AZ49" s="3"/>
-      <c r="BA49" s="3"/>
-      <c r="BB49" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:AA1"/>
+    <mergeCell ref="A1:W1"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>